<commit_message>
started with the problem def
</commit_message>
<xml_diff>
--- a/__ConferenceStuff/Conference options and choice.xlsx
+++ b/__ConferenceStuff/Conference options and choice.xlsx
@@ -600,8 +600,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Team Document" ma:contentTypeID="0x010100A35317DCC28344A7B82488658A034A5C010046233E0BD084A74DB18247B09BDD9753" ma:contentTypeVersion="6" ma:contentTypeDescription=" " ma:contentTypeScope="" ma:versionID="75afdf903140e6a1b6a74513f6a78a8e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c18b97ec-0207-4827-9b53-3cd5cea07467" xmlns:ns3="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7" xmlns:ns5="39750d87-7e17-441a-9113-4df334e06b56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c788368599872cfb0e40fccc0158f476" ns2:_="" ns3:_="" ns5:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Team Document" ma:contentTypeID="0x010100A35317DCC28344A7B82488658A034A5C010046233E0BD084A74DB18247B09BDD9753" ma:contentTypeVersion="7" ma:contentTypeDescription=" " ma:contentTypeScope="" ma:versionID="cb37e81710481e51c418888f1b749a99">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c18b97ec-0207-4827-9b53-3cd5cea07467" xmlns:ns3="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7" xmlns:ns5="39750d87-7e17-441a-9113-4df334e06b56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9fc5335b274709d67a1a8c890b6d48d2" ns2:_="" ns3:_="" ns5:_="">
     <xsd:import namespace="c18b97ec-0207-4827-9b53-3cd5cea07467"/>
     <xsd:import namespace="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7"/>
     <xsd:import namespace="39750d87-7e17-441a-9113-4df334e06b56"/>
@@ -628,6 +628,7 @@
                 <xsd:element ref="ns5:MediaServiceAutoTags" minOccurs="0"/>
                 <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceOCR" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -778,6 +779,13 @@
     <xsd:element name="MediaServiceAutoTags" ma:index="28" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="31" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -983,23 +991,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{700C1011-1C93-43CE-9CFA-0B0787E341B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c18b97ec-0207-4827-9b53-3cd5cea07467"/>
-    <ds:schemaRef ds:uri="2f6a910d-138e-42c1-8e8a-320c1b7cf3f7"/>
-    <ds:schemaRef ds:uri="39750d87-7e17-441a-9113-4df334e06b56"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDE71BE6-D079-4BA4-BD0E-F83A6DD453F7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>